<commit_message>
Excel z rodzajami dokumentow uzupełnionymi o typy edycji (do ponownego zaimportowania do słonia)
</commit_message>
<xml_diff>
--- a/SQL/Rodzaje_dokumentow_Eteczka.xlsx
+++ b/SQL/Rodzaje_dokumentow_Eteczka.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eteczka.main\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\eAD_Git\SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="157">
   <si>
     <t>A</t>
   </si>
@@ -461,10 +461,43 @@
     <t>ZapOdo</t>
   </si>
   <si>
-    <t>aa</t>
-  </si>
-  <si>
     <t>eAd</t>
+  </si>
+  <si>
+    <t>symbol</t>
+  </si>
+  <si>
+    <t>nazwa</t>
+  </si>
+  <si>
+    <t>dokwlasny</t>
+  </si>
+  <si>
+    <t>teczkadzial</t>
+  </si>
+  <si>
+    <t>firma</t>
+  </si>
+  <si>
+    <t>pracownik</t>
+  </si>
+  <si>
+    <t>datadokumentu</t>
+  </si>
+  <si>
+    <t>datapocz</t>
+  </si>
+  <si>
+    <t>datakoniec</t>
+  </si>
+  <si>
+    <t>typ 1</t>
+  </si>
+  <si>
+    <t>typ2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">firma </t>
   </si>
 </sst>
 </file>
@@ -796,22 +829,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E70"/>
+  <dimension ref="A1:P70"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A51" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E1" sqref="E1:E70"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G2" sqref="G2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21.85546875" customWidth="1"/>
     <col min="2" max="2" width="43.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="3" max="3" width="4" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="4.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="12.85546875" customWidth="1"/>
+    <col min="14" max="14" width="15.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>88</v>
       </c>
@@ -821,14 +860,44 @@
       <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" t="s">
-        <v>144</v>
+      <c r="D1">
+        <v>1</v>
       </c>
       <c r="E1" t="s">
+        <v>144</v>
+      </c>
+      <c r="G1" t="s">
+        <v>155</v>
+      </c>
+      <c r="H1" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I1" t="s">
+        <v>146</v>
+      </c>
+      <c r="J1" t="s">
+        <v>147</v>
+      </c>
+      <c r="K1" t="s">
+        <v>148</v>
+      </c>
+      <c r="L1" t="s">
+        <v>149</v>
+      </c>
+      <c r="M1" t="s">
+        <v>150</v>
+      </c>
+      <c r="N1" t="s">
+        <v>151</v>
+      </c>
+      <c r="O1" t="s">
+        <v>152</v>
+      </c>
+      <c r="P1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>72</v>
       </c>
@@ -838,14 +907,35 @@
       <c r="C2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
-        <v>144</v>
+      <c r="D2">
+        <v>1</v>
       </c>
       <c r="E2" t="s">
+        <v>144</v>
+      </c>
+      <c r="G2" t="s">
+        <v>154</v>
+      </c>
+      <c r="H2" t="s">
         <v>145</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="I2" t="s">
+        <v>146</v>
+      </c>
+      <c r="J2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K2" t="s">
+        <v>148</v>
+      </c>
+      <c r="L2" t="s">
+        <v>156</v>
+      </c>
+      <c r="M2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>73</v>
       </c>
@@ -855,14 +945,14 @@
       <c r="C3" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>144</v>
+      <c r="D3">
+        <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>75</v>
       </c>
@@ -872,14 +962,14 @@
       <c r="C4" t="s">
         <v>0</v>
       </c>
-      <c r="D4" t="s">
-        <v>144</v>
+      <c r="D4">
+        <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>76</v>
       </c>
@@ -889,14 +979,14 @@
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="s">
-        <v>144</v>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -906,14 +996,14 @@
       <c r="C6" t="s">
         <v>3</v>
       </c>
-      <c r="D6" t="s">
-        <v>144</v>
+      <c r="D6">
+        <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>78</v>
       </c>
@@ -923,14 +1013,14 @@
       <c r="C7" t="s">
         <v>3</v>
       </c>
-      <c r="D7" t="s">
-        <v>144</v>
+      <c r="D7">
+        <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>79</v>
       </c>
@@ -940,14 +1030,14 @@
       <c r="C8" t="s">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>144</v>
+      <c r="D8">
+        <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>80</v>
       </c>
@@ -957,14 +1047,14 @@
       <c r="C9" t="s">
         <v>0</v>
       </c>
-      <c r="D9" t="s">
-        <v>144</v>
+      <c r="D9">
+        <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>81</v>
       </c>
@@ -974,14 +1064,14 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
-      <c r="D10" t="s">
-        <v>144</v>
+      <c r="D10">
+        <v>1</v>
       </c>
       <c r="E10" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>82</v>
       </c>
@@ -991,14 +1081,14 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
-      <c r="D11" t="s">
-        <v>144</v>
+      <c r="D11">
+        <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>86</v>
       </c>
@@ -1008,14 +1098,14 @@
       <c r="C12" t="s">
         <v>83</v>
       </c>
-      <c r="D12" t="s">
-        <v>144</v>
+      <c r="D12">
+        <v>1</v>
       </c>
       <c r="E12" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>84</v>
       </c>
@@ -1025,14 +1115,14 @@
       <c r="C13" t="s">
         <v>83</v>
       </c>
-      <c r="D13" t="s">
-        <v>144</v>
+      <c r="D13">
+        <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>85</v>
       </c>
@@ -1042,14 +1132,14 @@
       <c r="C14" t="s">
         <v>83</v>
       </c>
-      <c r="D14" t="s">
-        <v>144</v>
+      <c r="D14">
+        <v>1</v>
       </c>
       <c r="E14" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>142</v>
       </c>
@@ -1059,14 +1149,14 @@
       <c r="C15" t="s">
         <v>83</v>
       </c>
-      <c r="D15" t="s">
-        <v>144</v>
+      <c r="D15">
+        <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" ht="30" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>143</v>
       </c>
@@ -1076,11 +1166,11 @@
       <c r="C16" t="s">
         <v>83</v>
       </c>
-      <c r="D16" t="s">
-        <v>144</v>
+      <c r="D16">
+        <v>1</v>
       </c>
       <c r="E16" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1093,11 +1183,11 @@
       <c r="C17" t="s">
         <v>83</v>
       </c>
-      <c r="D17" t="s">
-        <v>144</v>
+      <c r="D17">
+        <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,11 +1200,11 @@
       <c r="C18" t="s">
         <v>83</v>
       </c>
-      <c r="D18" t="s">
-        <v>144</v>
+      <c r="D18">
+        <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="19" spans="1:5" ht="29.25" x14ac:dyDescent="0.25">
@@ -1127,11 +1217,11 @@
       <c r="C19" t="s">
         <v>83</v>
       </c>
-      <c r="D19" t="s">
-        <v>144</v>
+      <c r="D19">
+        <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1144,11 +1234,11 @@
       <c r="C20" t="s">
         <v>83</v>
       </c>
-      <c r="D20" t="s">
-        <v>144</v>
+      <c r="D20">
+        <v>1</v>
       </c>
       <c r="E20" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1161,11 +1251,11 @@
       <c r="C21" t="s">
         <v>83</v>
       </c>
-      <c r="D21" t="s">
-        <v>144</v>
+      <c r="D21">
+        <v>1</v>
       </c>
       <c r="E21" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1178,11 +1268,11 @@
       <c r="C22" t="s">
         <v>83</v>
       </c>
-      <c r="D22" t="s">
-        <v>144</v>
+      <c r="D22">
+        <v>1</v>
       </c>
       <c r="E22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1195,11 +1285,11 @@
       <c r="C23" t="s">
         <v>83</v>
       </c>
-      <c r="D23" t="s">
-        <v>144</v>
+      <c r="D23">
+        <v>1</v>
       </c>
       <c r="E23" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1212,11 +1302,11 @@
       <c r="C24" t="s">
         <v>83</v>
       </c>
-      <c r="D24" t="s">
-        <v>144</v>
+      <c r="D24">
+        <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1229,11 +1319,11 @@
       <c r="C25" t="s">
         <v>83</v>
       </c>
-      <c r="D25" t="s">
-        <v>144</v>
+      <c r="D25">
+        <v>2</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1246,11 +1336,11 @@
       <c r="C26" t="s">
         <v>83</v>
       </c>
-      <c r="D26" t="s">
-        <v>144</v>
+      <c r="D26">
+        <v>2</v>
       </c>
       <c r="E26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1263,11 +1353,11 @@
       <c r="C27" t="s">
         <v>83</v>
       </c>
-      <c r="D27" t="s">
-        <v>144</v>
+      <c r="D27">
+        <v>2</v>
       </c>
       <c r="E27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1280,11 +1370,11 @@
       <c r="C28" t="s">
         <v>83</v>
       </c>
-      <c r="D28" t="s">
-        <v>144</v>
+      <c r="D28">
+        <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1297,11 +1387,11 @@
       <c r="C29" t="s">
         <v>83</v>
       </c>
-      <c r="D29" t="s">
-        <v>144</v>
+      <c r="D29">
+        <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1314,11 +1404,11 @@
       <c r="C30" t="s">
         <v>83</v>
       </c>
-      <c r="D30" t="s">
-        <v>144</v>
+      <c r="D30">
+        <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1331,11 +1421,11 @@
       <c r="C31" t="s">
         <v>83</v>
       </c>
-      <c r="D31" t="s">
-        <v>144</v>
+      <c r="D31">
+        <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1348,11 +1438,11 @@
       <c r="C32" t="s">
         <v>140</v>
       </c>
-      <c r="D32" t="s">
-        <v>144</v>
+      <c r="D32">
+        <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1365,11 +1455,11 @@
       <c r="C33" t="s">
         <v>83</v>
       </c>
-      <c r="D33" t="s">
-        <v>144</v>
+      <c r="D33">
+        <v>1</v>
       </c>
       <c r="E33" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1382,11 +1472,11 @@
       <c r="C34" t="s">
         <v>83</v>
       </c>
-      <c r="D34" t="s">
-        <v>144</v>
+      <c r="D34">
+        <v>1</v>
       </c>
       <c r="E34" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1399,11 +1489,11 @@
       <c r="C35" t="s">
         <v>83</v>
       </c>
-      <c r="D35" t="s">
-        <v>144</v>
+      <c r="D35">
+        <v>1</v>
       </c>
       <c r="E35" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1416,11 +1506,11 @@
       <c r="C36" t="s">
         <v>140</v>
       </c>
-      <c r="D36" t="s">
-        <v>144</v>
+      <c r="D36">
+        <v>1</v>
       </c>
       <c r="E36" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1433,11 +1523,11 @@
       <c r="C37" t="s">
         <v>140</v>
       </c>
-      <c r="D37" t="s">
-        <v>144</v>
+      <c r="D37">
+        <v>1</v>
       </c>
       <c r="E37" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1450,11 +1540,11 @@
       <c r="C38" t="s">
         <v>140</v>
       </c>
-      <c r="D38" t="s">
-        <v>144</v>
+      <c r="D38">
+        <v>1</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1467,11 +1557,11 @@
       <c r="C39" t="s">
         <v>140</v>
       </c>
-      <c r="D39" t="s">
-        <v>144</v>
+      <c r="D39">
+        <v>1</v>
       </c>
       <c r="E39" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -1484,11 +1574,11 @@
       <c r="C40" t="s">
         <v>83</v>
       </c>
-      <c r="D40" t="s">
-        <v>144</v>
+      <c r="D40">
+        <v>1</v>
       </c>
       <c r="E40" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1501,11 +1591,11 @@
       <c r="C41" t="s">
         <v>83</v>
       </c>
-      <c r="D41" t="s">
-        <v>144</v>
+      <c r="D41">
+        <v>1</v>
       </c>
       <c r="E41" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1518,11 +1608,11 @@
       <c r="C42" t="s">
         <v>83</v>
       </c>
-      <c r="D42" t="s">
-        <v>144</v>
+      <c r="D42">
+        <v>1</v>
       </c>
       <c r="E42" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1535,11 +1625,11 @@
       <c r="C43" t="s">
         <v>83</v>
       </c>
-      <c r="D43" t="s">
-        <v>144</v>
+      <c r="D43">
+        <v>1</v>
       </c>
       <c r="E43" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1552,11 +1642,11 @@
       <c r="C44" t="s">
         <v>83</v>
       </c>
-      <c r="D44" t="s">
-        <v>144</v>
+      <c r="D44">
+        <v>1</v>
       </c>
       <c r="E44" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1569,11 +1659,11 @@
       <c r="C45" t="s">
         <v>83</v>
       </c>
-      <c r="D45" t="s">
-        <v>144</v>
+      <c r="D45">
+        <v>1</v>
       </c>
       <c r="E45" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1586,11 +1676,11 @@
       <c r="C46" t="s">
         <v>83</v>
       </c>
-      <c r="D46" t="s">
-        <v>144</v>
+      <c r="D46">
+        <v>1</v>
       </c>
       <c r="E46" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1603,11 +1693,11 @@
       <c r="C47" t="s">
         <v>83</v>
       </c>
-      <c r="D47" t="s">
-        <v>144</v>
+      <c r="D47">
+        <v>1</v>
       </c>
       <c r="E47" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -1620,11 +1710,11 @@
       <c r="C48" t="s">
         <v>83</v>
       </c>
-      <c r="D48" t="s">
-        <v>144</v>
+      <c r="D48">
+        <v>1</v>
       </c>
       <c r="E48" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1637,11 +1727,11 @@
       <c r="C49" t="s">
         <v>83</v>
       </c>
-      <c r="D49" t="s">
-        <v>144</v>
+      <c r="D49">
+        <v>1</v>
       </c>
       <c r="E49" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="50" spans="1:5" ht="30" x14ac:dyDescent="0.25">
@@ -1654,11 +1744,11 @@
       <c r="C50" t="s">
         <v>83</v>
       </c>
-      <c r="D50" t="s">
-        <v>144</v>
+      <c r="D50">
+        <v>1</v>
       </c>
       <c r="E50" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1671,11 +1761,11 @@
       <c r="C51" t="s">
         <v>83</v>
       </c>
-      <c r="D51" t="s">
-        <v>144</v>
+      <c r="D51">
+        <v>2</v>
       </c>
       <c r="E51" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1688,11 +1778,11 @@
       <c r="C52" t="s">
         <v>83</v>
       </c>
-      <c r="D52" t="s">
-        <v>144</v>
+      <c r="D52">
+        <v>1</v>
       </c>
       <c r="E52" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1705,11 +1795,11 @@
       <c r="C53" t="s">
         <v>83</v>
       </c>
-      <c r="D53" t="s">
-        <v>144</v>
+      <c r="D53">
+        <v>1</v>
       </c>
       <c r="E53" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1722,11 +1812,11 @@
       <c r="C54" t="s">
         <v>83</v>
       </c>
-      <c r="D54" t="s">
-        <v>144</v>
+      <c r="D54">
+        <v>1</v>
       </c>
       <c r="E54" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1739,11 +1829,11 @@
       <c r="C55" t="s">
         <v>83</v>
       </c>
-      <c r="D55" t="s">
-        <v>144</v>
+      <c r="D55">
+        <v>1</v>
       </c>
       <c r="E55" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1756,11 +1846,11 @@
       <c r="C56" t="s">
         <v>83</v>
       </c>
-      <c r="D56" t="s">
-        <v>144</v>
+      <c r="D56">
+        <v>1</v>
       </c>
       <c r="E56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1773,11 +1863,11 @@
       <c r="C57" t="s">
         <v>83</v>
       </c>
-      <c r="D57" t="s">
-        <v>144</v>
+      <c r="D57">
+        <v>1</v>
       </c>
       <c r="E57" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1790,11 +1880,11 @@
       <c r="C58" t="s">
         <v>83</v>
       </c>
-      <c r="D58" t="s">
-        <v>144</v>
+      <c r="D58">
+        <v>1</v>
       </c>
       <c r="E58" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1807,11 +1897,11 @@
       <c r="C59" t="s">
         <v>83</v>
       </c>
-      <c r="D59" t="s">
-        <v>144</v>
+      <c r="D59">
+        <v>1</v>
       </c>
       <c r="E59" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -1824,11 +1914,11 @@
       <c r="C60" t="s">
         <v>83</v>
       </c>
-      <c r="D60" t="s">
-        <v>144</v>
+      <c r="D60">
+        <v>1</v>
       </c>
       <c r="E60" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -1841,11 +1931,11 @@
       <c r="C61" t="s">
         <v>83</v>
       </c>
-      <c r="D61" t="s">
-        <v>144</v>
+      <c r="D61">
+        <v>1</v>
       </c>
       <c r="E61" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1858,11 +1948,11 @@
       <c r="C62" t="s">
         <v>83</v>
       </c>
-      <c r="D62" t="s">
-        <v>144</v>
+      <c r="D62">
+        <v>1</v>
       </c>
       <c r="E62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1875,11 +1965,11 @@
       <c r="C63" t="s">
         <v>83</v>
       </c>
-      <c r="D63" t="s">
-        <v>144</v>
+      <c r="D63">
+        <v>2</v>
       </c>
       <c r="E63" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1892,11 +1982,11 @@
       <c r="C64" t="s">
         <v>83</v>
       </c>
-      <c r="D64" t="s">
-        <v>144</v>
+      <c r="D64">
+        <v>2</v>
       </c>
       <c r="E64" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1909,11 +1999,11 @@
       <c r="C65" t="s">
         <v>83</v>
       </c>
-      <c r="D65" t="s">
-        <v>144</v>
+      <c r="D65">
+        <v>1</v>
       </c>
       <c r="E65" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1926,11 +2016,11 @@
       <c r="C66" t="s">
         <v>83</v>
       </c>
-      <c r="D66" t="s">
-        <v>144</v>
+      <c r="D66">
+        <v>1</v>
       </c>
       <c r="E66" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1943,11 +2033,11 @@
       <c r="C67" t="s">
         <v>83</v>
       </c>
-      <c r="D67" t="s">
-        <v>144</v>
+      <c r="D67">
+        <v>1</v>
       </c>
       <c r="E67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1960,11 +2050,11 @@
       <c r="C68" t="s">
         <v>83</v>
       </c>
-      <c r="D68" t="s">
-        <v>144</v>
+      <c r="D68">
+        <v>1</v>
       </c>
       <c r="E68" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1977,11 +2067,11 @@
       <c r="C69" t="s">
         <v>83</v>
       </c>
-      <c r="D69" t="s">
-        <v>144</v>
+      <c r="D69">
+        <v>2</v>
       </c>
       <c r="E69" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1994,11 +2084,11 @@
       <c r="C70" t="s">
         <v>83</v>
       </c>
-      <c r="D70" t="s">
-        <v>144</v>
+      <c r="D70">
+        <v>1</v>
       </c>
       <c r="E70" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
   </sheetData>

</xml_diff>